<commit_message>
Added Example for Sandbox apic
</commit_message>
<xml_diff>
--- a/examples/L3OUT_eBGP.xlsx
+++ b/examples/L3OUT_eBGP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graber/Documents/python/ACI-L3OUT-Modular-gitHub/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298E48C2-E546-CA4C-9D57-45DA034C880A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2A87C5-3863-6742-870D-900BA99A27C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="2440" windowWidth="26440" windowHeight="14800" xr2:uid="{236C4CF3-AB4C-0147-B4E6-28D5CB909C90}"/>
   </bookViews>
@@ -135,18 +135,6 @@
     <t>10.8.73.110</t>
   </si>
   <si>
-    <t>10.8.153.74</t>
-  </si>
-  <si>
-    <t>10.8.153.75</t>
-  </si>
-  <si>
-    <t>10.8.153.76</t>
-  </si>
-  <si>
-    <t>10.8.153.77</t>
-  </si>
-  <si>
     <t>L3OUT-TEST1</t>
   </si>
   <si>
@@ -157,6 +145,18 @@
   </si>
   <si>
     <t>TEST2</t>
+  </si>
+  <si>
+    <t>10.8.75.98</t>
+  </si>
+  <si>
+    <t>10.8.75.102</t>
+  </si>
+  <si>
+    <t>10.8.75.106</t>
+  </si>
+  <si>
+    <t>10.8.75.110</t>
   </si>
 </sst>
 </file>
@@ -519,14 +519,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02C9E000-98C0-4A42-9160-CE4D9727BF95}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.6640625" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
     <col min="12" max="12" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -614,7 +615,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
@@ -626,7 +627,7 @@
         <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s">
         <v>28</v>
@@ -688,7 +689,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
@@ -700,7 +701,7 @@
         <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
         <v>28</v>
@@ -715,37 +716,37 @@
         <v>111</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="M4">
         <v>112</v>
       </c>
       <c r="N4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="O4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="Q4">
         <v>211</v>
       </c>
       <c r="R4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="S4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="U4">
         <v>212</v>
       </c>
       <c r="V4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="W4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>